<commit_message>
chore: update cleanup-gh-pages pages
</commit_message>
<xml_diff>
--- a/cleanup-gh-pages/StructureDefinition-mii-pr-diagnose-condition.xlsx
+++ b/cleanup-gh-pages/StructureDefinition-mii-pr-diagnose-condition.xlsx
@@ -60,7 +60,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2025-03-31</t>
+    <t>2025-12-12</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -1494,10 +1494,10 @@
 </t>
   </si>
   <si>
-    <t>Fall oder Kontakt</t>
-  </si>
-  <si>
-    <t>Fall oder Kontakt, bei dem die Diagnose festgestellt wurde.</t>
+    <t>Kontakt (Aufenthaltsbezug)</t>
+  </si>
+  <si>
+    <t>Kontakt, während dem die Diagnose erstellt wurde oder mit dem die Diagnose in Zusammenhang steht.</t>
   </si>
   <si>
     <t>This will typically be the encounter the event occurred within, but some activities may be initiated prior to or after the official completion of an encounter but still be tied to the context of the encounter. This record indicates the encounter this particular record is associated with.  In the case of a "new" diagnosis reflecting ongoing/revised information about the condition, this might be distinct from the first encounter in which the underlying condition was first "known".</t>

</xml_diff>